<commit_message>
Lettura valori filtri dai files
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/InputFiles/Forecast.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/InputFiles/Forecast.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fperrino\Desktop\KPI UT_LAVORO_LEFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B764E30E-0B2B-4416-8890-7907B6BC788A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{CE016E61-7459-40AD-BB52-464C55DF94A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,19 +505,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986F63D4-D872-476B-A8DF-A86C3916F277}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +592,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Renaming a ordinamento alfabetico filtri
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/InputFiles/Forecast.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/InputFiles/Forecast.xlsx
@@ -568,7 +568,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4:Y15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -761,35 +763,27 @@
         <v>101</v>
       </c>
       <c r="Z4">
-        <f>Y4+1</f>
         <v>102</v>
       </c>
       <c r="AA4">
-        <f t="shared" ref="AA4:AG4" si="0">Z4+1</f>
         <v>103</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="0"/>
         <v>106</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="0"/>
         <v>109</v>
       </c>
     </row>
@@ -864,39 +858,30 @@
         <v>97</v>
       </c>
       <c r="Y5">
-        <f>Y4+10</f>
         <v>111</v>
       </c>
       <c r="Z5">
-        <f>Z4+10</f>
         <v>112</v>
       </c>
       <c r="AA5">
-        <f t="shared" ref="AA5:AG5" si="1">AA4+10</f>
         <v>113</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="1"/>
         <v>114</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="1"/>
         <v>115</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="1"/>
         <v>118</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="1"/>
         <v>119</v>
       </c>
     </row>
@@ -971,39 +956,30 @@
         <v>97</v>
       </c>
       <c r="Y6">
-        <f t="shared" ref="Y6:Y8" si="2">Y5+10</f>
         <v>121</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:AG7" si="3">Z5+10</f>
         <v>122</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="3"/>
         <v>129</v>
       </c>
     </row>
@@ -1078,39 +1054,30 @@
         <v>97</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="2"/>
         <v>131</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="3"/>
         <v>133</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="3"/>
         <v>134</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="3"/>
         <v>137</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="3"/>
         <v>138</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="3"/>
         <v>139</v>
       </c>
     </row>
@@ -1185,39 +1152,30 @@
         <v>97</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="2"/>
         <v>141</v>
       </c>
       <c r="Z8">
-        <f>Y8+1</f>
         <v>142</v>
       </c>
       <c r="AA8">
-        <f t="shared" ref="AA8" si="4">Z8+1</f>
         <v>143</v>
       </c>
       <c r="AB8">
-        <f t="shared" ref="AB8" si="5">AA8+1</f>
         <v>144</v>
       </c>
       <c r="AC8">
-        <f t="shared" ref="AC8" si="6">AB8+1</f>
         <v>145</v>
       </c>
       <c r="AD8">
-        <f t="shared" ref="AD8" si="7">AC8+1</f>
         <v>146</v>
       </c>
       <c r="AE8">
-        <f t="shared" ref="AE8" si="8">AD8+1</f>
         <v>147</v>
       </c>
       <c r="AF8">
-        <f t="shared" ref="AF8" si="9">AE8+1</f>
         <v>148</v>
       </c>
       <c r="AG8">
-        <f t="shared" ref="AG8" si="10">AF8+1</f>
         <v>149</v>
       </c>
     </row>
@@ -1292,39 +1250,30 @@
         <v>97</v>
       </c>
       <c r="Y9">
-        <f>Y8+10</f>
         <v>151</v>
       </c>
       <c r="Z9">
-        <f>Z8+10</f>
         <v>152</v>
       </c>
       <c r="AA9">
-        <f t="shared" ref="AA9:AG9" si="11">AA8+10</f>
         <v>153</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="11"/>
         <v>154</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="11"/>
         <v>155</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="11"/>
         <v>156</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="11"/>
         <v>157</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="11"/>
         <v>158</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="11"/>
         <v>159</v>
       </c>
     </row>
@@ -1399,39 +1348,30 @@
         <v>97</v>
       </c>
       <c r="Y10">
-        <f t="shared" ref="Y10:AG12" si="12">Y9+10</f>
         <v>161</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="12"/>
         <v>162</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="12"/>
         <v>163</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="12"/>
         <v>164</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="12"/>
         <v>165</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="12"/>
         <v>166</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="12"/>
         <v>167</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="12"/>
         <v>168</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="12"/>
         <v>169</v>
       </c>
     </row>
@@ -1506,39 +1446,30 @@
         <v>97</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="12"/>
         <v>171</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="12"/>
         <v>172</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="12"/>
         <v>173</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="12"/>
         <v>174</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="12"/>
         <v>175</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="12"/>
         <v>176</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="12"/>
         <v>177</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="12"/>
         <v>178</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="12"/>
         <v>179</v>
       </c>
     </row>
@@ -1613,39 +1544,30 @@
         <v>97</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="12"/>
         <v>181</v>
       </c>
       <c r="Z12">
-        <f>Y12+1</f>
         <v>182</v>
       </c>
       <c r="AA12">
-        <f t="shared" ref="AA12" si="13">Z12+1</f>
         <v>183</v>
       </c>
       <c r="AB12">
-        <f t="shared" ref="AB12" si="14">AA12+1</f>
         <v>184</v>
       </c>
       <c r="AC12">
-        <f t="shared" ref="AC12" si="15">AB12+1</f>
         <v>185</v>
       </c>
       <c r="AD12">
-        <f t="shared" ref="AD12" si="16">AC12+1</f>
         <v>186</v>
       </c>
       <c r="AE12">
-        <f t="shared" ref="AE12" si="17">AD12+1</f>
         <v>187</v>
       </c>
       <c r="AF12">
-        <f t="shared" ref="AF12" si="18">AE12+1</f>
         <v>188</v>
       </c>
       <c r="AG12">
-        <f t="shared" ref="AG12" si="19">AF12+1</f>
         <v>189</v>
       </c>
     </row>
@@ -1720,39 +1642,30 @@
         <v>97</v>
       </c>
       <c r="Y13">
-        <f>Y12+10</f>
         <v>191</v>
       </c>
       <c r="Z13">
-        <f>Z12+10</f>
         <v>192</v>
       </c>
       <c r="AA13">
-        <f t="shared" ref="AA13:AG13" si="20">AA12+10</f>
         <v>193</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="20"/>
         <v>194</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="20"/>
         <v>195</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="20"/>
         <v>196</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="20"/>
         <v>197</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="20"/>
         <v>198</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="20"/>
         <v>199</v>
       </c>
     </row>
@@ -1827,39 +1740,30 @@
         <v>97</v>
       </c>
       <c r="Y14">
-        <f t="shared" ref="Y14:AG15" si="21">Y13+10</f>
         <v>201</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="21"/>
         <v>202</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="21"/>
         <v>203</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="21"/>
         <v>204</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="21"/>
         <v>205</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="21"/>
         <v>206</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="21"/>
         <v>207</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="21"/>
         <v>208</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="21"/>
         <v>209</v>
       </c>
     </row>
@@ -1934,39 +1838,30 @@
         <v>97</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="21"/>
         <v>211</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="21"/>
         <v>212</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="21"/>
         <v>213</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="21"/>
         <v>214</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="21"/>
         <v>215</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="21"/>
         <v>216</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="21"/>
         <v>217</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="21"/>
         <v>218</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="21"/>
         <v>219</v>
       </c>
     </row>

</xml_diff>